<commit_message>
ajustes gráfico e código
</commit_message>
<xml_diff>
--- a/Gráficos/Novo Tempo de execução.xlsx
+++ b/Gráficos/Novo Tempo de execução.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Algoritmo Brute Force" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Algoritmo Árvore de Sufixos" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="Planilha1" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Algoritmo Árvore de Sufixos 100" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Planilha1" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="222">
   <si>
     <t xml:space="preserve">Tamanho da Entrada</t>
   </si>
@@ -514,6 +515,171 @@
   </si>
   <si>
     <t xml:space="preserve">QCJSMJGYZZJYDGGFSOBYVOLTPMFWRWACTEYBRBGGZHEFGLTRDJKNNINLXTAPPSOHRFYTOOQYJHSIKDIFYRBKOLNQRBJVEOYEZDJYKIKWWXCXKANMRPWIEACPUASDCMEWWFDWQJISRWOMTSKGDXYBDOUVYIWXKXAHZBXEHEJURLNEAITJARHDGNEFARYFEOABZILHWCNHVZJUVBOATCRWZEXGVHIYNXGVAPJLWHKUCVWQLCPZFPKZFYRDKYKCIJMXLELOWEOJPHAQGPVQHJCZXMUOHAERUSCANUVAWGFSRLDHTNEGGFTUIMENSLQEOVNARAPGVFXTYIFDSZFLMPXCFSLXXRBXABPFIGVNLACJLZNUIHHHGJDRHFEYMTQUDAUOJVOWQAHJPNFPOICXUUXSTCUAOKZIBTOPXBUOBDEDXOOCAYQHVZKNLKXMDBHRIFXUZLLYLEEJEYTNJNGAZWDMGXGZKUIUTUPEMWVNYHZHBLENJGLILIKKVCPTVAGTBDYUOWWIWTYLLBRWVVXHGOJXVHQXCNVACJHEEKSWABZEUAYJHSBIKEIGJVVEATBMYKEWXZPZCBCPJCTCGTFJITZHEHSXUOTDKLXQWPZJPSMIAJBZBTJZCOHEDZCIYRLKXSYEAKRSJWRPZRONRVTSZVMELIBQKYMFBWXTYORNSEMDBVEIVOJGFWERBEQZPNNSRKEGBBCTVDMMXSDAQIRIJINERSARVPSSUQZNIVZSFTHWFLJQXLPWMMBXYVJJXRRZJNYGIQYGEPNGPWSLGSXSZRGERHDZQPEBFPQVVGZFEAAEYFISESMRXWWKRLMZPYTPKHFLKXZECOQJIBRSKPGNWTRDDSMKRFVBCUURQTWHMQXZIFNAXADEPYJZQUVAFQLXGMIHWGLIHDFEUPYDUMZFMORXFMXZOLBKCIJZDAYWEDBHWMZAOPQEUGNCETTGWXQXHJNBHEEGWXTCSTGUAQOUZSEVYVFFUPEYYXRTRJFIUOBBWJLXEWVDAJZHISZXJMZZKJOEXCLEMIXTTWURFVGLEGLRDZXKILHKGSUDWXYVTJZYOOPUWQLPFLBUIHFMMUINPSAYYSKRFINAECJHECDLUBBNMXRKIDJWURCFSWUMNQLMZLXDYHYQLVEHYVNWBVCTLMQLJWIWTAPCEOLYRDFQZNOELJUGSVKVFKKEGIZUOOGLYBKCGTCFSPWKUHYDWLKVXIQAIHAJNISMGJELYIQQVWOHLMGKJSCAGFSALQNLBEOSLKVFKJDRDLPWHAFFEHYINPCKOJKIDKVNPHBTKCOIFVZJPXRYOOWNFENHIVBATYFQBPWMHRHGQVZQIGAXYOGSZFZFEZQIMECQJMEIYKFRMHLRXRTATYRMEBTKUVEODYVLSXIFWBOBSJISJTDCUEAOOQYNMCJGLSYDCQUEQAEDMYCWFZIGGHXIURJMILMFHRKVSUDLXDXHPFQKZJXWLZDYMLPJIGHGMILNRAGMAQFKZAILOUWOGDWMMAWXTNZBBWYTRMFALVXSDIILPFTWCAOWJJBLBTMOPLRAFZMVXSGHUQGATPWXIOHZMPVFFPRZNZEDBWMSGTEWYEGTLEZCVCWCXAUTLEAUPZDNGZWJUUELAPPEUQSLIVFKRSXDPWSHGCAAIVSCAYIVKUOTZQTOEVRMGCQBPENITLEOQVZKTKEITRLDOVZPXIGKFHXMZDWHPAHRXVHNPYAOFWVAUWSZOUXWUYCHOPLENKYRYHOCSDSYDSWNZTJMDRMWYYDQHZIZUEWZEUIXXMUKUMCYOEHIVFXNSPRXJTLCNYVVGVDCKVTMZVRFZPUUSYYSDDUMYUUVVJNBZXDQUTBHTCRLZGUHTQVVAHVWFXPDYJRDNPCFSKBXSFFMNZQZLHPWXYNQVOMRRYMKBTEZFLYQPGHQDBBEOKKKZUSOTHGQABCGEPCUKJYJUGGWUBBLZONJEMUSAZLYZEGDNKMPAUNQWWVKEYJSOIKTWBNAUNVHXTIYLTBFIZWMZMOKCENBKYASSLPKUCWSHQSATWMCWFYBCNTNQWFWTAHBPDBZQPQNHCAVMKZWHAJVMAOMZCFCCFVNFSKENOVOKYYFGYWFFNILXJPNSTVJMSXMMYUJVHLQWKATWCYWUMHRIJYECOVLMGHKZVQUVJMUKTOFBNLCBCMWZBDXEZTCPKEPCGOQAJXSAEARSWCNPEXMZXXAIHIKXEKAKCATTFGITXQLITLFGWCZASIDZEYGXEKNBQOLRYCUMHFKGWFAYJZGPWKGPHINLVEOFVPBGDAOJUVBTGULADATVQNKDJFIPCWMZFFNNLKHHVOWGWEYONDWZJZCVSLLMZAIAUDYBMUQWPEVMVBFHOJUQHAXQDMMJPCQONBMZQXDDUHGJBCDRHEXVFGNHXTAMOPOPBILRWCQEZQYQBDZQCYFYROJOEXHLJVNOQOUTXVUKPAUQULFKBJFSECJOZKHJZPPPTRTHKBBAEXUYKOXPILNZXJTDDVDXWVILXPKZTKPFMIIJYJAGFMCRCEYOYWBZLIQTOMEKQMZYEZQEMGECGKMPIFUDQRYIVOGARXSSENZMHWWYNBNZEETWCYVNGYAYLXZZRYQEKBZYWPLDCVFAMOICASTVZTXBJMTZWAKATQWCQMUSBFNDPDVRRUHCGSQDLPWLSHMCQTARXRVVEJXQJJLMAOQPGFVBMHUFOCOHLUKYNNUZYMBNXTCJPFMETKHTPMQCFTXYIEICVAUMFGFUBPCVTJDCHAWQQVBBKJCBCAGMITHEBFDQJCOXAWLZJLWAUWMJOAPQWYPTIVPTCHWDBUSONWPRWZGKWVGJTDEOKIDSCQZYLQFFOCCNTFYDYIQFKMAMVEDPPSBLHGPNRKDMMODXURHQWSUSZTLVFCJAOMBLLZGOGLINZXHXHQBPDLLUCRWQKXLKDTLYJVATUDYDKNMAOMPJJJJMZIEAEWDCWCCYOLVNXHEZWCRQAQYOSBSTFLZZUSVLYJGACJGZJDSGRIIOIQVMXPB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000074</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000137</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000030</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000174</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000040</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000248</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000058</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000301</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000386</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000473</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000096</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000550</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000696</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000122</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000156</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000881</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000161</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000907</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000951</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.001018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000165</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.001084</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.001157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000163</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.001225</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.001298</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.001334</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.001407</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000166</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.001466</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.001498</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000219</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.001585</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.001647</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.001694</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000189</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.001751</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000236</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.001822</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000266</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.001925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.001987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000264</t>
   </si>
   <si>
     <t xml:space="preserve">Observação:</t>
@@ -897,7 +1063,7 @@
   </sheetPr>
   <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F64" activeCellId="0" sqref="F64"/>
     </sheetView>
   </sheetViews>
@@ -905,7 +1071,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="25.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="25.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="15.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="109.89"/>
@@ -1778,7 +1944,7 @@
   </sheetPr>
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
@@ -2588,9 +2754,821 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:F51"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="16.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="15.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="109.89"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="n">
+        <v>100</v>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="n">
+        <v>200</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="n">
+        <v>300</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>400</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="n">
+        <v>500</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="n">
+        <v>600</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="n">
+        <v>700</v>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="n">
+        <v>800</v>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="n">
+        <v>900</v>
+      </c>
+      <c r="B10" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="B11" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="n">
+        <v>1100</v>
+      </c>
+      <c r="B12" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="n">
+        <v>1200</v>
+      </c>
+      <c r="B13" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="n">
+        <v>1300</v>
+      </c>
+      <c r="B14" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="n">
+        <v>1400</v>
+      </c>
+      <c r="B15" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="n">
+        <v>1500</v>
+      </c>
+      <c r="B16" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="n">
+        <v>1600</v>
+      </c>
+      <c r="B17" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="n">
+        <v>1700</v>
+      </c>
+      <c r="B18" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="n">
+        <v>1800</v>
+      </c>
+      <c r="B19" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="n">
+        <v>1900</v>
+      </c>
+      <c r="B20" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="n">
+        <v>2000</v>
+      </c>
+      <c r="B21" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="n">
+        <v>2100</v>
+      </c>
+      <c r="B22" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="n">
+        <v>2200</v>
+      </c>
+      <c r="B23" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="n">
+        <v>2300</v>
+      </c>
+      <c r="B24" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="n">
+        <v>2400</v>
+      </c>
+      <c r="B25" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="n">
+        <v>2500</v>
+      </c>
+      <c r="B26" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="n">
+        <v>2600</v>
+      </c>
+      <c r="B27" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="n">
+        <v>2700</v>
+      </c>
+      <c r="B28" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="n">
+        <v>2800</v>
+      </c>
+      <c r="B29" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5" t="n">
+        <v>2900</v>
+      </c>
+      <c r="B30" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="n">
+        <v>3000</v>
+      </c>
+      <c r="B31" s="5" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="n">
+        <v>3100</v>
+      </c>
+      <c r="B32" s="5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5" t="n">
+        <v>3200</v>
+      </c>
+      <c r="B33" s="5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="5" t="n">
+        <v>3300</v>
+      </c>
+      <c r="B34" s="5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5" t="n">
+        <v>3400</v>
+      </c>
+      <c r="B35" s="5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="5" t="n">
+        <v>3500</v>
+      </c>
+      <c r="B36" s="5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="5" t="n">
+        <v>3600</v>
+      </c>
+      <c r="B37" s="5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="5" t="n">
+        <v>3700</v>
+      </c>
+      <c r="B38" s="5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5" t="n">
+        <v>3800</v>
+      </c>
+      <c r="B39" s="5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="5" t="n">
+        <v>3900</v>
+      </c>
+      <c r="B40" s="5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5" t="n">
+        <v>4000</v>
+      </c>
+      <c r="B41" s="5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="5" t="n">
+        <v>4100</v>
+      </c>
+      <c r="B42" s="5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="5" t="n">
+        <v>4200</v>
+      </c>
+      <c r="B43" s="5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="5" t="n">
+        <v>4300</v>
+      </c>
+      <c r="B44" s="5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="5" t="n">
+        <v>4400</v>
+      </c>
+      <c r="B45" s="5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="5" t="n">
+        <v>4500</v>
+      </c>
+      <c r="B46" s="5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="5" t="n">
+        <v>4600</v>
+      </c>
+      <c r="B47" s="5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="5" t="n">
+        <v>4700</v>
+      </c>
+      <c r="B48" s="5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="5" t="n">
+        <v>4800</v>
+      </c>
+      <c r="B49" s="5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="5" t="n">
+        <v>4900</v>
+      </c>
+      <c r="B50" s="5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="5" t="n">
+        <v>5000</v>
+      </c>
+      <c r="B51" s="5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -2602,15 +3580,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>164</v>
+        <v>219</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>165</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>166</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update graphics and code
</commit_message>
<xml_diff>
--- a/Gráficos/Novo Tempo de execução.xlsx
+++ b/Gráficos/Novo Tempo de execução.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Algoritmo Brute Force" sheetId="1" state="visible" r:id="rId3"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="242">
   <si>
     <t xml:space="preserve">Tamanho da Entrada</t>
   </si>
@@ -43,124 +43,184 @@
     <t xml:space="preserve">Substring Utilizada</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0030</t>
+    <t xml:space="preserve">0.0008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QYELJZSDIFFZENLRBOIQWXPZOSMGLAXBYEPIDJNNOUNSHYLKPVANTPMHIZNTZLWXRNHUWWJNQYFZZTKQOMDHEQROPGJOTFNKVXGR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0054</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0172</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FFE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0757</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1290</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.2078</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.3006</t>
   </si>
   <si>
     <t xml:space="preserve">0.0006</t>
   </si>
   <si>
-    <t xml:space="preserve">QY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QYELJZSDIFFZENLRBOIQWXPZOSMGLAXBYEPIDJNNOUNSHYLKPVANTPMHIZNTZLWXRNHUWWJNQYFZZTKQOMDHEQROPGJOTFNKVXGR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KSWKNGVQZWGZSDWROWUTUBPNDAAJCONMIJWYSTORPURIAPBQLVJFYBUCDVNFLCRVOPTGIKZYGQIGHJXUHIBFLYJPVWWGBQDPFXXQHWONPYWWHV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0031</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CBABSYBMVQTMOXHJIEXXATJBDTNELJONMPQENTRJJMVAJELSKIPNDAOITDMGOBUAQMHFIAORMLTWSEOEOFRTHHCCNOIDPEGHTNNBNDSBPOXJUNNJUHEBQGFF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0066 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0015 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0050 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0019 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IWB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0022 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">QS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0072 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0024 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0136 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0053 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">WXR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0082 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">YB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0144 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0029 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">TE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0128</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0040</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YI</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.0380 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0130 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">FFE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18.0193</t>
+    <t xml:space="preserve">0.4292</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5820</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7756</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0051</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.0786</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3811</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.6662</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0158</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.3295</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.6001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.3389</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0053</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.6474</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.5854</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0513</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.4063</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0354</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.1034</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.5761</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0463</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.2961</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0749</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.3127</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0443</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.0586</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8352</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.4286</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0409</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.8581</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0042</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.3522</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0622</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14.5126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17.5305</t>
   </si>
   <si>
     <t xml:space="preserve">0.0075</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JMEUJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DDRZCUARYIHDTFLUQBXYWEPRNPRSNQDQTURWQSPOCXTYEEUUFRUDWMXLBQEOGJHZFYXVQPLVOEVSIPOQIKTGWSSYIYOOHVQMUPJMEUJSYEMIVCYENUKJMEJXEYLLTDZPTICZCLUCQGLLJLRWFEHUIRRNREAKICADKCCPPWTHDETOQMMXQTTZMKODROQZQQCDUGULDNTIUOWKAKJRFDSSPIXGYNHRFJUBQQNVDGDZUBJWLVPQAHKPPIYOVFFBPBCHRRCWXFWTIHSTEHLEPWWGGUWBZDEOEJXXABWAISVQBNJGVXKMTGSZARCCUJQZUQYWRUWAOSQQFCWCZIOURJVTAZVUIOVEEWBXQXZFRQXXUVBTDQPWZKSBJNXUDVYJRZHJZGOQYNPSIRNOHCMIMELYSISVDQFWSOGRUWHTKXNUOBIXDVHSZUQTCIPIAWESKKJGJTBTQPNGSYFXTOPUIHOMPFUSDBMNNYVWRXPJOFRGDWDYMVUUCKGURDMUEAJRYFOREFASMTAPRFPDCMXFWGZQJNKPPWGOBWFHEIBQBBIVIZYLLYSKGTAPGMGXIOLLLTSPDTHGWPBHPASAAKKGFMXLZDIHRWTERNVUJDCFSEMHGGKGSWOXJLKKOVRHTMMKAJGJMIQFMFOUNYCIXQHGBSQRPJBKYNUAYCJLKBSZGITWJWEGOLOQFEJWPKGNZCPYEYLRCDQKNLGWJKCYYQQDWZAOKIDLLTJRTUIVZYGNMOLVZQTZILCHLEXXPAIAVURPOCMQAUFMJSKKIFJRRNACUXBJZJLVDEMUGYMJTRXEJHOSNZLEMNIGKJRJUEEAJQUPRGYMZWQKFGCSFPYRCGAOPTYMYEMHXIYQQZCPXUZCAEXFVVWACYQTSOFQVTZUDXKTYMKVGMAISXNPSLPWKGQEWXWTTVNWUZQVNCQVOQDIPQYICNEOVWUUWQPPNFLJEDESGVNWNRFDJDNLSTBQSVMOLBFAGSKLWOFELSCBLJGVOTIJOKZIFNWTODVXWFKSWPYHJAIVMOQAJYJAIKIQXHLMKGLGOVAKKYRTBCONSGNEFZEPJOHHXUVIBGQPBRZLRSGUUXJPDZTKYZCHNJQLELVHRNYUGXHYROUOLEDQDWBBVFKKOBVUOSBIGBCMYKMSYHGLNJDQHGTCLFMCIKWXEAFKBHZCRNWRUCEHLIZUOSWCYKEGWCFBCKNGUMKLAGFWKJGXRFRIANKYXQGWSOXXYKDSZPGZXLXHWDEQJVYJKKJHARDSFCPGNUAMLGNITMRQQVIBQIMASVKUOPOWUGCHACVOLKYEWQWONEPGMBGGYSCPKRLEXNNZRKNCWOJUEHJROAXCEGLCANRMEESBTHBLTQPPEAMKIVEYXDABJLGMZZYDETHXAIIWAALHAXRKUVISZJVKWBYVBXBFSICUSNQSNEZNDTYYQISPRNCORALSZMXRUBOOQEHDIITODTMUBGLVVNJMOWEPJDHFHXUXBDDMLWAPROLUWWPRKAGAXMPGSYNZVHYZKBLYZNPQDALZWCSGDAGANYIHWVISFGTPKENJTECWEPXBRRHUSQWHOGOMCWGJEZYOFOYYSCWXRTAINHFHZDOPKECOCKXIKXXPLXOGZKFSGFAVOHCQLSFVYJLCUIKGFJVTGLZHYGZGLCBBLDRWVZTVIEXEOHKUTIPZTQJRWKXJMYKYDEWADQVNWSSLCEHVMYWIOHZKSZTEXFEDJBDMTBCRVWEXANUPLTXZAYJSXEZXKDAVGFIZGKRCGVBIJYZURWWTVHOUMNRYSTTZZDYFPRJXPLIALHWEGSXDALXOAROTKJSJNSREMCEDPMDAVZEBUEEWPCMSTALFJFRYZKFNMJQCXVESXJURNAPEEBWZBJFMQWNSISFUDYYATDUQMQJBRYHXZGXCPCPIAECIWJEBHDDBGXTUQDVHBCGBIDFAHWKHAMRYVWZDZCGHCZBSEYBGAHJLLOLSLVCNJVMERLJSQRBSRCKVALDDSMOFDBAOYCBHXPNRBXLRONLHRVFUIIXCXNKAOKQMOTTNJIEKFSDWHQFYNKSVVRZUEJUSTMGJFBXOKDAPVDNCTTDGDXDAPFUTOQOKCUTIWQWGWXXRCLWYGZGLYMMNRIJHZXRDTNLRFKZBJZTNMRLSSUDQIRGZAPGBOAEJNQDSCCULBPYNIMFAILSQCYREPZFFZKPOCSHEWDRYUPNEDVELIYBKZSPOSWWTGLIKFRQBWHBSZRWCOCQWARGZMXQGUOBCZJPGCFJYPNQOEMSSOIQRCYSOWKWSYXWZJNFLTRKKECAKPSEFBUWDSPTQZPKAOJZXWFLRWVBCZBMOWQWXMSCEJXXLOHLCSKCPRNIPKKRJNFAJVWIHQMOCJLNXUACNMEEETMVDYPMMUOXSMIBDUPFGCUDZWFMILQOEEKHDZWRTMQNZYPEVELBJHGIDOWLZMCGQMPVNNMIADWZDLFYRQBCXIKAWGNXUPDNDTISIVBIAZJDKOCDEDGDNSDLZTJVKOIOJRGSOJCQIMTUCXYHDGMQYQEZLPVVDFJPYSJMBLCKZYECVELYMXRLPVMAKJWNPHENZNCDBGPAEVEAAPAMNRZCMMFWXBMMISCKIENJMELRZQTZFVOUNNZBBEYZHMNRERBMXQXKUJDUBWVGRJDGZEICKIDRWRKCKMRIEOSBZVXATSJMEMTDSDFCNLVJCFNOTEWYTOBSLYVESERWSMBKRJMEUJPYOCMIJJIEZLWLJTRDXKAPWDZPMNTIWKGNPVXYGHCFSASDUKGTUIJTOKICAELYQTLFQKFWRJCJMWOIGVBBFMWTZEWZIJZZENGVXORPZVALSPVYMZBRNXNMELNOUPPACYVZMPONKPZCGWDSXGLLGYZMJPAFEQGGODFCSUPDLQHRPMLMVWXBVXNGOPOSHWYXZDZSZRXMHEFWTQJONIRKHGSVVGNDENAERCWSTVFAZKZSBKIQUZCCFWZBFPGJCGNTILOBGTEIFFCIRLYLKCPQZRTGGZPKFFGQSUTZNZJSGLBXWBLJGCBHTUNBTCMAJSSCMMDBNMTUZWRYAEHGHIPCCCEXGQXQISSWEVXRJSLIRFGRLNZSXOVBQZYWRYOBQIXWFWPOO</t>
   </si>
   <si>
     <t xml:space="preserve">0.000322</t>
@@ -1061,10 +1121,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F87"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F64" activeCellId="0" sqref="F64"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1102,7 +1162,7 @@
         <v>100</v>
       </c>
       <c r="B2" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -1119,10 +1179,10 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="n">
-        <v>110</v>
+        <v>200</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>10</v>
@@ -1133,799 +1193,598 @@
       <c r="E3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="n">
-        <v>120</v>
+        <v>300</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="n">
-        <v>130</v>
+        <v>400</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="n">
-        <v>140</v>
+        <v>500</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="n">
-        <v>150</v>
+        <v>600</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="n">
-        <v>160</v>
+        <v>700</v>
       </c>
       <c r="B8" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
-        <v>170</v>
+        <v>800</v>
       </c>
       <c r="B9" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="n">
-        <v>180</v>
+        <v>900</v>
       </c>
       <c r="B10" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="n">
-        <v>190</v>
+        <v>1000</v>
       </c>
       <c r="B11" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="n">
-        <v>200</v>
+        <v>1100</v>
       </c>
       <c r="B12" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="n">
-        <v>300</v>
+        <v>1200</v>
       </c>
       <c r="B13" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="n">
-        <v>310</v>
+        <v>1300</v>
       </c>
       <c r="B14" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="n">
-        <v>320</v>
+        <v>1400</v>
       </c>
       <c r="B15" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="n">
-        <v>330</v>
+        <v>1500</v>
       </c>
       <c r="B16" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="n">
-        <v>340</v>
+        <v>1600</v>
       </c>
       <c r="B17" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="n">
-        <v>350</v>
+        <v>1700</v>
       </c>
       <c r="B18" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="n">
-        <v>360</v>
+        <v>1800</v>
       </c>
       <c r="B19" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="n">
-        <v>370</v>
+        <v>1900</v>
       </c>
       <c r="B20" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="n">
-        <v>380</v>
+        <v>2000</v>
       </c>
       <c r="B21" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5" t="n">
-        <v>390</v>
+        <v>2100</v>
       </c>
       <c r="B22" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="n">
-        <v>400</v>
+        <v>2200</v>
       </c>
       <c r="B23" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="n">
-        <v>410</v>
+        <v>2300</v>
       </c>
       <c r="B24" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="n">
-        <v>420</v>
+        <v>2400</v>
       </c>
       <c r="B25" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="n">
-        <v>430</v>
+        <v>2500</v>
       </c>
       <c r="B26" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="n">
-        <v>440</v>
+        <v>2600</v>
       </c>
       <c r="B27" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="n">
-        <v>450</v>
+        <v>2700</v>
       </c>
       <c r="B28" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="n">
-        <v>460</v>
+        <v>2800</v>
       </c>
       <c r="B29" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="n">
-        <v>470</v>
+        <v>2900</v>
       </c>
       <c r="B30" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="n">
-        <v>480</v>
+        <v>3000</v>
       </c>
       <c r="B31" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="n">
-        <v>490</v>
+        <v>3100</v>
       </c>
       <c r="B32" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="n">
-        <v>500</v>
+        <v>3200</v>
       </c>
       <c r="B33" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="n">
-        <v>510</v>
+        <v>3300</v>
       </c>
       <c r="B34" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="n">
-        <v>520</v>
+        <v>3400</v>
       </c>
       <c r="B35" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="n">
-        <v>530</v>
+        <v>3500</v>
       </c>
       <c r="B36" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="n">
-        <v>540</v>
+        <v>3600</v>
       </c>
       <c r="B37" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="n">
-        <v>550</v>
+        <v>3700</v>
       </c>
       <c r="B38" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5" t="n">
-        <v>560</v>
+        <v>3800</v>
       </c>
       <c r="B39" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5" t="n">
-        <v>570</v>
+        <v>3900</v>
       </c>
       <c r="B40" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="n">
-        <v>580</v>
+        <v>4000</v>
       </c>
       <c r="B41" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="n">
-        <v>590</v>
+        <v>4100</v>
       </c>
       <c r="B42" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="n">
-        <v>600</v>
+        <v>4200</v>
       </c>
       <c r="B43" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5" t="n">
-        <v>700</v>
+        <v>4300</v>
       </c>
       <c r="B44" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5" t="n">
-        <v>800</v>
+        <v>4400</v>
       </c>
       <c r="B45" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5" t="n">
-        <v>900</v>
+        <v>4500</v>
       </c>
       <c r="B46" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="5" t="n">
-        <v>1000</v>
+        <v>4600</v>
       </c>
       <c r="B47" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="5" t="n">
-        <v>1100</v>
+        <v>4700</v>
       </c>
       <c r="B48" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="n">
-        <v>1200</v>
+        <v>4800</v>
       </c>
       <c r="B49" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="5" t="n">
-        <v>1300</v>
+        <v>4900</v>
       </c>
       <c r="B50" s="5" t="n">
-        <v>5</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="5" t="n">
-        <v>1400</v>
+        <v>5000</v>
       </c>
       <c r="B51" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="n">
-        <v>1500</v>
-      </c>
-      <c r="B52" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5" t="n">
-        <v>1600</v>
-      </c>
-      <c r="B53" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="5" t="n">
-        <v>1700</v>
-      </c>
-      <c r="B54" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="5" t="n">
-        <v>1800</v>
-      </c>
-      <c r="B55" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="5" t="n">
-        <v>1900</v>
-      </c>
-      <c r="B56" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="n">
-        <v>2000</v>
-      </c>
-      <c r="B57" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="5" t="n">
-        <v>2100</v>
-      </c>
-      <c r="B58" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="5" t="n">
-        <v>2200</v>
-      </c>
-      <c r="B59" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="5" t="n">
-        <v>2300</v>
-      </c>
-      <c r="B60" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="5" t="n">
-        <v>2400</v>
-      </c>
-      <c r="B61" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="5" t="n">
-        <v>2500</v>
-      </c>
-      <c r="B62" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="5" t="n">
-        <v>2600</v>
-      </c>
-      <c r="B63" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="5" t="n">
-        <v>2700</v>
-      </c>
-      <c r="B64" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="5" t="n">
-        <v>2800</v>
-      </c>
-      <c r="B65" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="5" t="n">
-        <v>2900</v>
-      </c>
-      <c r="B66" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="5" t="n">
-        <v>3000</v>
-      </c>
-      <c r="B67" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="5" t="n">
-        <v>3100</v>
-      </c>
-      <c r="B68" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="5" t="n">
-        <v>3200</v>
-      </c>
-      <c r="B69" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="5" t="n">
-        <v>3300</v>
-      </c>
-      <c r="B70" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="5" t="n">
-        <v>3400</v>
-      </c>
-      <c r="B71" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="5" t="n">
-        <v>3500</v>
-      </c>
-      <c r="B72" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="5" t="n">
-        <v>3600</v>
-      </c>
-      <c r="B73" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="5" t="n">
-        <v>3700</v>
-      </c>
-      <c r="B74" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="5" t="n">
-        <v>3800</v>
-      </c>
-      <c r="B75" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="5" t="n">
-        <v>3900</v>
-      </c>
-      <c r="B76" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="5" t="n">
-        <v>4000</v>
-      </c>
-      <c r="B77" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="5" t="n">
-        <v>4100</v>
-      </c>
-      <c r="B78" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="5" t="n">
-        <v>4200</v>
-      </c>
-      <c r="B79" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="5" t="n">
-        <v>4300</v>
-      </c>
-      <c r="B80" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="5" t="n">
-        <v>4400</v>
-      </c>
-      <c r="B81" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="5" t="n">
-        <v>4500</v>
-      </c>
-      <c r="B82" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="5" t="n">
-        <v>4600</v>
-      </c>
-      <c r="B83" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="5" t="n">
-        <v>4700</v>
-      </c>
-      <c r="B84" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="5" t="n">
-        <v>4800</v>
-      </c>
-      <c r="B85" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="5" t="n">
-        <v>4900</v>
-      </c>
-      <c r="B86" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="5" t="n">
-        <v>5000</v>
-      </c>
-      <c r="B87" s="5" t="n">
-        <v>5</v>
-      </c>
-    </row>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1986,16 +1845,16 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2006,16 +1865,16 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2026,16 +1885,16 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2046,16 +1905,16 @@
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2066,16 +1925,16 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2086,16 +1945,16 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2106,16 +1965,16 @@
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2126,16 +1985,16 @@
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2146,16 +2005,16 @@
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2166,16 +2025,16 @@
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>81</v>
+        <v>101</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2186,16 +2045,16 @@
         <v>5</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2206,16 +2065,16 @@
         <v>5</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2226,16 +2085,16 @@
         <v>5</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2246,16 +2105,16 @@
         <v>5</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2266,16 +2125,16 @@
         <v>5</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2286,16 +2145,16 @@
         <v>5</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2306,16 +2165,16 @@
         <v>5</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2326,16 +2185,16 @@
         <v>5</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2346,16 +2205,16 @@
         <v>5</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2366,16 +2225,16 @@
         <v>5</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2386,16 +2245,16 @@
         <v>5</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2406,16 +2265,16 @@
         <v>5</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2426,16 +2285,16 @@
         <v>5</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2446,16 +2305,16 @@
         <v>5</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2466,16 +2325,16 @@
         <v>5</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2486,16 +2345,16 @@
         <v>5</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2506,16 +2365,16 @@
         <v>5</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2526,16 +2385,16 @@
         <v>5</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>152</v>
+        <v>172</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>155</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2546,16 +2405,16 @@
         <v>5</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2566,16 +2425,16 @@
         <v>5</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2756,7 +2615,7 @@
   </sheetPr>
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -2798,16 +2657,16 @@
         <v>1000</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2818,16 +2677,16 @@
         <v>1000</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2838,16 +2697,16 @@
         <v>1000</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2858,16 +2717,16 @@
         <v>1000</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>171</v>
+        <v>191</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2878,16 +2737,16 @@
         <v>1000</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>171</v>
+        <v>191</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2898,16 +2757,16 @@
         <v>1000</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2918,16 +2777,16 @@
         <v>1000</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2938,16 +2797,16 @@
         <v>1000</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2958,16 +2817,16 @@
         <v>1000</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2978,16 +2837,16 @@
         <v>1000</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>182</v>
+        <v>202</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2998,16 +2857,16 @@
         <v>1000</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>183</v>
+        <v>203</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3018,16 +2877,16 @@
         <v>1000</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>90</v>
+        <v>110</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3038,16 +2897,16 @@
         <v>1000</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3058,16 +2917,16 @@
         <v>1000</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3078,16 +2937,16 @@
         <v>1000</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3098,16 +2957,16 @@
         <v>1000</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3118,16 +2977,16 @@
         <v>1000</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3138,16 +2997,16 @@
         <v>1000</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3158,16 +3017,16 @@
         <v>1000</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>198</v>
+        <v>218</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3178,16 +3037,16 @@
         <v>1000</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>201</v>
+        <v>221</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3198,16 +3057,16 @@
         <v>1000</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>202</v>
+        <v>222</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>203</v>
+        <v>223</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3218,16 +3077,16 @@
         <v>1000</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>204</v>
+        <v>224</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3238,16 +3097,16 @@
         <v>1000</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>206</v>
+        <v>226</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>207</v>
+        <v>227</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3258,16 +3117,16 @@
         <v>1000</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3278,16 +3137,16 @@
         <v>1000</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>209</v>
+        <v>229</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3298,16 +3157,16 @@
         <v>1000</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>210</v>
+        <v>230</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3318,16 +3177,16 @@
         <v>1000</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>212</v>
+        <v>232</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3338,16 +3197,16 @@
         <v>1000</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>214</v>
+        <v>234</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>215</v>
+        <v>235</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>155</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3358,16 +3217,16 @@
         <v>1000</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>216</v>
+        <v>236</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3378,16 +3237,16 @@
         <v>1000</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>218</v>
+        <v>238</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3580,15 +3439,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>219</v>
+        <v>239</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>220</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>